<commit_message>
new alignment 2020-1965 and 2020-pre1964
</commit_message>
<xml_diff>
--- a/Microgastrine_classifications.xlsx
+++ b/Microgastrine_classifications.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33800" yWindow="-1460" windowWidth="27300" windowHeight="16140" activeTab="3"/>
+    <workbookView xWindow="28880" yWindow="1320" windowWidth="33120" windowHeight="21640" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Test" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="concat" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="212">
   <si>
     <t>Microgaster Latreille</t>
   </si>
@@ -660,13 +661,28 @@
   </si>
   <si>
     <t>Dodogaster Rousse</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; "2020.Microgastrine"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [dir=back]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"2020.Microgastrine" -&gt; </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -705,8 +721,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -740,6 +762,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -799,7 +827,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -835,6 +863,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1165,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42:F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1561,43 +1592,43 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="36" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="C28" s="6" t="s">
+    <row r="28" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="37"/>
+      <c r="C28" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="36" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="6" t="s">
+    <row r="29" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="36" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2247,8 +2278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3354,7 +3385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
@@ -3876,10 +3907,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CF14"/>
+  <dimension ref="A1:CF17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:AM17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4730,6 +4761,1814 @@
         <v>99</v>
       </c>
     </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AE17" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AF17" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="AG17" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="AH17" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AI17" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ17" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="AK17" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="AL17" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM17" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8:J45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="52" customWidth="1"/>
+    <col min="7" max="7" width="43.5" customWidth="1"/>
+    <col min="16" max="16" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1">
+        <v>2020</v>
+      </c>
+      <c r="D1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" t="str">
+        <f>_xlfn.CONCAT(B1,C1,D1,A1,E1)</f>
+        <v>"2020.Larissimus_Nixon"</v>
+      </c>
+      <c r="H1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J1" t="str">
+        <f>_xlfn.CONCAT(F1,H1)</f>
+        <v>"2020.Larissimus_Nixon" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P1" t="s">
+        <v>211</v>
+      </c>
+      <c r="R1" t="s">
+        <v>210</v>
+      </c>
+      <c r="S1" t="str">
+        <f>_xlfn.CONCAT(P1,F1,R1)</f>
+        <v>"2020.Microgastrine" -&gt; "2020.Larissimus_Nixon" [dir=back]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2">
+        <v>2020</v>
+      </c>
+      <c r="D2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F45" si="0">_xlfn.CONCAT(B2,C2,D2,A2,E2)</f>
+        <v>"2020.Alloplitis_Nixon"</v>
+      </c>
+      <c r="H2" t="s">
+        <v>209</v>
+      </c>
+      <c r="J2" t="str">
+        <f t="shared" ref="J2:J45" si="1">_xlfn.CONCAT(F2,H2)</f>
+        <v>"2020.Alloplitis_Nixon" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P2" t="s">
+        <v>211</v>
+      </c>
+      <c r="R2" t="s">
+        <v>210</v>
+      </c>
+      <c r="S2" t="str">
+        <f>_xlfn.CONCAT(P2,F2,R2)</f>
+        <v>"2020.Microgastrine" -&gt; "2020.Alloplitis_Nixon" [dir=back]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3">
+        <v>2020</v>
+      </c>
+      <c r="D3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Philoplitis_Nixon"</v>
+      </c>
+      <c r="H3" t="s">
+        <v>209</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Philoplitis_Nixon" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P3" t="s">
+        <v>211</v>
+      </c>
+      <c r="R3" t="s">
+        <v>210</v>
+      </c>
+      <c r="S3" t="str">
+        <f t="shared" ref="S3:S45" si="2">_xlfn.CONCAT(P3,F3,R3)</f>
+        <v>"2020.Microgastrine" -&gt; "2020.Philoplitis_Nixon" [dir=back]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4">
+        <v>2020</v>
+      </c>
+      <c r="D4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Prasmodon_Nixon"</v>
+      </c>
+      <c r="H4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Prasmodon_Nixon" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P4" t="s">
+        <v>211</v>
+      </c>
+      <c r="R4" t="s">
+        <v>210</v>
+      </c>
+      <c r="S4" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Prasmodon_Nixon" [dir=back]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5">
+        <v>2020</v>
+      </c>
+      <c r="D5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Semionis_Nixon"</v>
+      </c>
+      <c r="H5" t="s">
+        <v>209</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Semionis_Nixon" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P5" t="s">
+        <v>211</v>
+      </c>
+      <c r="R5" t="s">
+        <v>210</v>
+      </c>
+      <c r="S5" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Semionis_Nixon" [dir=back]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6">
+        <v>2020</v>
+      </c>
+      <c r="D6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Sendaphne_Nixon"</v>
+      </c>
+      <c r="H6" t="s">
+        <v>209</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Sendaphne_Nixon" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P6" t="s">
+        <v>211</v>
+      </c>
+      <c r="R6" t="s">
+        <v>210</v>
+      </c>
+      <c r="S6" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Sendaphne_Nixon" [dir=back]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7">
+        <v>2020</v>
+      </c>
+      <c r="D7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E7" t="s">
+        <v>208</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Parenion_Nixon"</v>
+      </c>
+      <c r="H7" t="s">
+        <v>209</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Parenion_Nixon" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P7" t="s">
+        <v>211</v>
+      </c>
+      <c r="R7" t="s">
+        <v>210</v>
+      </c>
+      <c r="S7" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Parenion_Nixon" [dir=back]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8">
+        <v>2020</v>
+      </c>
+      <c r="D8" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Clarkinella_Mason"</v>
+      </c>
+      <c r="H8" t="s">
+        <v>209</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Clarkinella_Mason" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P8" t="s">
+        <v>211</v>
+      </c>
+      <c r="R8" t="s">
+        <v>210</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Clarkinella_Mason" [dir=back]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9">
+        <v>2020</v>
+      </c>
+      <c r="D9" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" t="s">
+        <v>208</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Papanteles_Mason"</v>
+      </c>
+      <c r="H9" t="s">
+        <v>209</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Papanteles_Mason" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P9" t="s">
+        <v>211</v>
+      </c>
+      <c r="R9" t="s">
+        <v>210</v>
+      </c>
+      <c r="S9" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Papanteles_Mason" [dir=back]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10">
+        <v>2020</v>
+      </c>
+      <c r="D10" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Pelicope_Mason"</v>
+      </c>
+      <c r="H10" t="s">
+        <v>209</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Pelicope_Mason" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P10" t="s">
+        <v>211</v>
+      </c>
+      <c r="R10" t="s">
+        <v>210</v>
+      </c>
+      <c r="S10" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Pelicope_Mason" [dir=back]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11">
+        <v>2020</v>
+      </c>
+      <c r="D11" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11" t="s">
+        <v>208</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Venanus_Mason"</v>
+      </c>
+      <c r="H11" t="s">
+        <v>209</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Venanus_Mason" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P11" t="s">
+        <v>211</v>
+      </c>
+      <c r="R11" t="s">
+        <v>210</v>
+      </c>
+      <c r="S11" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Venanus_Mason" [dir=back]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C12">
+        <v>2020</v>
+      </c>
+      <c r="D12" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" t="s">
+        <v>208</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Exulonyyx_Mason"</v>
+      </c>
+      <c r="H12" t="s">
+        <v>209</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Exulonyyx_Mason" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P12" t="s">
+        <v>211</v>
+      </c>
+      <c r="R12" t="s">
+        <v>210</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Exulonyyx_Mason" [dir=back]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13">
+        <v>2020</v>
+      </c>
+      <c r="D13" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13" t="s">
+        <v>208</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Napamus_Papp"</v>
+      </c>
+      <c r="H13" t="s">
+        <v>209</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Napamus_Papp" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P13" t="s">
+        <v>211</v>
+      </c>
+      <c r="R13" t="s">
+        <v>210</v>
+      </c>
+      <c r="S13" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Napamus_Papp" [dir=back]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C14">
+        <v>2020</v>
+      </c>
+      <c r="D14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" t="s">
+        <v>208</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Lathrapanteles_Williams"</v>
+      </c>
+      <c r="H14" t="s">
+        <v>209</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Lathrapanteles_Williams" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P14" t="s">
+        <v>211</v>
+      </c>
+      <c r="R14" t="s">
+        <v>210</v>
+      </c>
+      <c r="S14" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Lathrapanteles_Williams" [dir=back]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C15">
+        <v>2020</v>
+      </c>
+      <c r="D15" t="s">
+        <v>207</v>
+      </c>
+      <c r="E15" t="s">
+        <v>208</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Austrocotesia_Austin_and_Dangerfield"</v>
+      </c>
+      <c r="H15" t="s">
+        <v>209</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Austrocotesia_Austin_and_Dangerfield" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P15" t="s">
+        <v>211</v>
+      </c>
+      <c r="R15" t="s">
+        <v>210</v>
+      </c>
+      <c r="S15" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Austrocotesia_Austin_and_Dangerfield" [dir=back]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16">
+        <v>2020</v>
+      </c>
+      <c r="D16" t="s">
+        <v>207</v>
+      </c>
+      <c r="E16" t="s">
+        <v>208</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Neoclarkinella_Rema_and_Narendran"</v>
+      </c>
+      <c r="H16" t="s">
+        <v>209</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Neoclarkinella_Rema_and_Narendran" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P16" t="s">
+        <v>211</v>
+      </c>
+      <c r="R16" t="s">
+        <v>210</v>
+      </c>
+      <c r="S16" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Neoclarkinella_Rema_and_Narendran" [dir=back]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17">
+        <v>2020</v>
+      </c>
+      <c r="D17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Xanthapanteles_Whitfield"</v>
+      </c>
+      <c r="H17" t="s">
+        <v>209</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Xanthapanteles_Whitfield" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P17" t="s">
+        <v>211</v>
+      </c>
+      <c r="R17" t="s">
+        <v>210</v>
+      </c>
+      <c r="S17" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Xanthapanteles_Whitfield" [dir=back]</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" t="s">
+        <v>208</v>
+      </c>
+      <c r="C18">
+        <v>2020</v>
+      </c>
+      <c r="D18" t="s">
+        <v>207</v>
+      </c>
+      <c r="E18" t="s">
+        <v>208</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Pseudovenanides_Xiao_and_You"</v>
+      </c>
+      <c r="H18" t="s">
+        <v>209</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Pseudovenanides_Xiao_and_You" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P18" t="s">
+        <v>211</v>
+      </c>
+      <c r="R18" t="s">
+        <v>210</v>
+      </c>
+      <c r="S18" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Pseudovenanides_Xiao_and_You" [dir=back]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19">
+        <v>2020</v>
+      </c>
+      <c r="D19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E19" t="s">
+        <v>208</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Chaoa_Luo_and_You"</v>
+      </c>
+      <c r="H19" t="s">
+        <v>209</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Chaoa_Luo_and_You" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P19" t="s">
+        <v>211</v>
+      </c>
+      <c r="R19" t="s">
+        <v>210</v>
+      </c>
+      <c r="S19" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Chaoa_Luo_and_You" [dir=back]</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20">
+        <v>2020</v>
+      </c>
+      <c r="D20" t="s">
+        <v>207</v>
+      </c>
+      <c r="E20" t="s">
+        <v>208</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Cuneogaster_Choi_and_Whitfield"</v>
+      </c>
+      <c r="H20" t="s">
+        <v>209</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Cuneogaster_Choi_and_Whitfield" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P20" t="s">
+        <v>211</v>
+      </c>
+      <c r="R20" t="s">
+        <v>210</v>
+      </c>
+      <c r="S20" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Cuneogaster_Choi_and_Whitfield" [dir=back]</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C21">
+        <v>2020</v>
+      </c>
+      <c r="D21" t="s">
+        <v>207</v>
+      </c>
+      <c r="E21" t="s">
+        <v>208</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Kiwigaster_FernandezTriana_Whitifled_and_Ward"</v>
+      </c>
+      <c r="H21" t="s">
+        <v>209</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Kiwigaster_FernandezTriana_Whitifled_and_Ward" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P21" t="s">
+        <v>211</v>
+      </c>
+      <c r="R21" t="s">
+        <v>210</v>
+      </c>
+      <c r="S21" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Kiwigaster_FernandezTriana_Whitifled_and_Ward" [dir=back]</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22">
+        <v>2020</v>
+      </c>
+      <c r="D22" t="s">
+        <v>207</v>
+      </c>
+      <c r="E22" t="s">
+        <v>208</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Mariapanteles_Whitfield_and_Fernandez-Triana"</v>
+      </c>
+      <c r="H22" t="s">
+        <v>209</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Mariapanteles_Whitfield_and_Fernandez-Triana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P22" t="s">
+        <v>211</v>
+      </c>
+      <c r="R22" t="s">
+        <v>210</v>
+      </c>
+      <c r="S22" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Mariapanteles_Whitfield_and_Fernandez-Triana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" t="s">
+        <v>208</v>
+      </c>
+      <c r="C23">
+        <v>2020</v>
+      </c>
+      <c r="D23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E23" t="s">
+        <v>208</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Shireplitis_Fernandez-Triana_and_Ward"</v>
+      </c>
+      <c r="H23" t="s">
+        <v>209</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Shireplitis_Fernandez-Triana_and_Ward" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P23" t="s">
+        <v>211</v>
+      </c>
+      <c r="R23" t="s">
+        <v>210</v>
+      </c>
+      <c r="S23" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Shireplitis_Fernandez-Triana_and_Ward" [dir=back]</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B24" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24">
+        <v>2020</v>
+      </c>
+      <c r="D24" t="s">
+        <v>207</v>
+      </c>
+      <c r="E24" t="s">
+        <v>208</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Dodogaster_Rousse"</v>
+      </c>
+      <c r="H24" t="s">
+        <v>209</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Dodogaster_Rousse" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P24" t="s">
+        <v>211</v>
+      </c>
+      <c r="R24" t="s">
+        <v>210</v>
+      </c>
+      <c r="S24" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Dodogaster_Rousse" [dir=back]</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" t="s">
+        <v>208</v>
+      </c>
+      <c r="C25">
+        <v>2020</v>
+      </c>
+      <c r="D25" t="s">
+        <v>207</v>
+      </c>
+      <c r="E25" t="s">
+        <v>208</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Pseudofornicia_van_Achterberg"</v>
+      </c>
+      <c r="H25" t="s">
+        <v>209</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Pseudofornicia_van_Achterberg" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P25" t="s">
+        <v>211</v>
+      </c>
+      <c r="R25" t="s">
+        <v>210</v>
+      </c>
+      <c r="S25" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Pseudofornicia_van_Achterberg" [dir=back]</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" t="s">
+        <v>208</v>
+      </c>
+      <c r="C26">
+        <v>2020</v>
+      </c>
+      <c r="D26" t="s">
+        <v>207</v>
+      </c>
+      <c r="E26" t="s">
+        <v>208</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Keylimepie_Fernandez-Triana"</v>
+      </c>
+      <c r="H26" t="s">
+        <v>209</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Keylimepie_Fernandez-Triana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P26" t="s">
+        <v>211</v>
+      </c>
+      <c r="R26" t="s">
+        <v>210</v>
+      </c>
+      <c r="S26" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Keylimepie_Fernandez-Triana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B27" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27">
+        <v>2020</v>
+      </c>
+      <c r="D27" t="s">
+        <v>207</v>
+      </c>
+      <c r="E27" t="s">
+        <v>208</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Agupta_FernandezTriana"</v>
+      </c>
+      <c r="H27" t="s">
+        <v>209</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Agupta_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P27" t="s">
+        <v>211</v>
+      </c>
+      <c r="R27" t="s">
+        <v>210</v>
+      </c>
+      <c r="S27" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Agupta_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B28" t="s">
+        <v>208</v>
+      </c>
+      <c r="C28">
+        <v>2020</v>
+      </c>
+      <c r="D28" t="s">
+        <v>207</v>
+      </c>
+      <c r="E28" t="s">
+        <v>208</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Austinocotesia_FernandezTriana"</v>
+      </c>
+      <c r="H28" t="s">
+        <v>209</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Austinocotesia_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P28" t="s">
+        <v>211</v>
+      </c>
+      <c r="R28" t="s">
+        <v>210</v>
+      </c>
+      <c r="S28" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Austinocotesia_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29">
+        <v>2020</v>
+      </c>
+      <c r="D29" t="s">
+        <v>207</v>
+      </c>
+      <c r="E29" t="s">
+        <v>208</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Billmasonius_FernandezTriana"</v>
+      </c>
+      <c r="H29" t="s">
+        <v>209</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Billmasonius_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P29" t="s">
+        <v>211</v>
+      </c>
+      <c r="R29" t="s">
+        <v>210</v>
+      </c>
+      <c r="S29" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Billmasonius_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B30" t="s">
+        <v>208</v>
+      </c>
+      <c r="C30">
+        <v>2020</v>
+      </c>
+      <c r="D30" t="s">
+        <v>207</v>
+      </c>
+      <c r="E30" t="s">
+        <v>208</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Carlmuesebeckius_FernandezTriana"</v>
+      </c>
+      <c r="H30" t="s">
+        <v>209</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Carlmuesebeckius_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P30" t="s">
+        <v>211</v>
+      </c>
+      <c r="R30" t="s">
+        <v>210</v>
+      </c>
+      <c r="S30" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Carlmuesebeckius_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31">
+        <v>2020</v>
+      </c>
+      <c r="D31" t="s">
+        <v>207</v>
+      </c>
+      <c r="E31" t="s">
+        <v>208</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Eripnopelta_Xiong_van_Achterberg_and_Chen"</v>
+      </c>
+      <c r="H31" t="s">
+        <v>209</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Eripnopelta_Xiong_van_Achterberg_and_Chen" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P31" t="s">
+        <v>211</v>
+      </c>
+      <c r="R31" t="s">
+        <v>210</v>
+      </c>
+      <c r="S31" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Eripnopelta_Xiong_van_Achterberg_and_Chen" [dir=back]</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B32" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32">
+        <v>2020</v>
+      </c>
+      <c r="D32" t="s">
+        <v>207</v>
+      </c>
+      <c r="E32" t="s">
+        <v>208</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Gilbertnixonius_FernandezTriana"</v>
+      </c>
+      <c r="H32" t="s">
+        <v>209</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Gilbertnixonius_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P32" t="s">
+        <v>211</v>
+      </c>
+      <c r="R32" t="s">
+        <v>210</v>
+      </c>
+      <c r="S32" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Gilbertnixonius_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33" t="s">
+        <v>208</v>
+      </c>
+      <c r="C33">
+        <v>2020</v>
+      </c>
+      <c r="D33" t="s">
+        <v>207</v>
+      </c>
+      <c r="E33" t="s">
+        <v>208</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Janhalacaste_FernandezTriana"</v>
+      </c>
+      <c r="H33" t="s">
+        <v>209</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Janhalacaste_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P33" t="s">
+        <v>211</v>
+      </c>
+      <c r="R33" t="s">
+        <v>210</v>
+      </c>
+      <c r="S33" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Janhalacaste_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B34" t="s">
+        <v>208</v>
+      </c>
+      <c r="C34">
+        <v>2020</v>
+      </c>
+      <c r="D34" t="s">
+        <v>207</v>
+      </c>
+      <c r="E34" t="s">
+        <v>208</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Jenopappius_FernandezTriana"</v>
+      </c>
+      <c r="H34" t="s">
+        <v>209</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Jenopappius_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P34" t="s">
+        <v>211</v>
+      </c>
+      <c r="R34" t="s">
+        <v>210</v>
+      </c>
+      <c r="S34" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Jenopappius_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B35" t="s">
+        <v>208</v>
+      </c>
+      <c r="C35">
+        <v>2020</v>
+      </c>
+      <c r="D35" t="s">
+        <v>207</v>
+      </c>
+      <c r="E35" t="s">
+        <v>208</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Jimwhitfieldius_FernandezTriana"</v>
+      </c>
+      <c r="H35" t="s">
+        <v>209</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Jimwhitfieldius_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P35" t="s">
+        <v>211</v>
+      </c>
+      <c r="R35" t="s">
+        <v>210</v>
+      </c>
+      <c r="S35" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Jimwhitfieldius_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B36" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36">
+        <v>2020</v>
+      </c>
+      <c r="D36" t="s">
+        <v>207</v>
+      </c>
+      <c r="E36" t="s">
+        <v>208</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Kotenkosius_FernandezTriana"</v>
+      </c>
+      <c r="H36" t="s">
+        <v>209</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Kotenkosius_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P36" t="s">
+        <v>211</v>
+      </c>
+      <c r="R36" t="s">
+        <v>210</v>
+      </c>
+      <c r="S36" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Kotenkosius_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B37" t="s">
+        <v>208</v>
+      </c>
+      <c r="C37">
+        <v>2020</v>
+      </c>
+      <c r="D37" t="s">
+        <v>207</v>
+      </c>
+      <c r="E37" t="s">
+        <v>208</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Markshawius_FernandezTriana"</v>
+      </c>
+      <c r="H37" t="s">
+        <v>209</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Markshawius_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P37" t="s">
+        <v>211</v>
+      </c>
+      <c r="R37" t="s">
+        <v>210</v>
+      </c>
+      <c r="S37" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Markshawius_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B38" t="s">
+        <v>208</v>
+      </c>
+      <c r="C38">
+        <v>2020</v>
+      </c>
+      <c r="D38" t="s">
+        <v>207</v>
+      </c>
+      <c r="E38" t="s">
+        <v>208</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Notogaster_FernandezTriana_and_Ward"</v>
+      </c>
+      <c r="H38" t="s">
+        <v>209</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Notogaster_FernandezTriana_and_Ward" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P38" t="s">
+        <v>211</v>
+      </c>
+      <c r="R38" t="s">
+        <v>210</v>
+      </c>
+      <c r="S38" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Notogaster_FernandezTriana_and_Ward" [dir=back]</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B39" t="s">
+        <v>208</v>
+      </c>
+      <c r="C39">
+        <v>2020</v>
+      </c>
+      <c r="D39" t="s">
+        <v>207</v>
+      </c>
+      <c r="E39" t="s">
+        <v>208</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Ohenri_FernandezTriana"</v>
+      </c>
+      <c r="H39" t="s">
+        <v>209</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Ohenri_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P39" t="s">
+        <v>211</v>
+      </c>
+      <c r="R39" t="s">
+        <v>210</v>
+      </c>
+      <c r="S39" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Ohenri_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B40" t="s">
+        <v>208</v>
+      </c>
+      <c r="C40">
+        <v>2020</v>
+      </c>
+      <c r="D40" t="s">
+        <v>207</v>
+      </c>
+      <c r="E40" t="s">
+        <v>208</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Qrocodiledundee_FernandezTriana"</v>
+      </c>
+      <c r="H40" t="s">
+        <v>209</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Qrocodiledundee_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P40" t="s">
+        <v>211</v>
+      </c>
+      <c r="R40" t="s">
+        <v>210</v>
+      </c>
+      <c r="S40" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Qrocodiledundee_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B41" t="s">
+        <v>208</v>
+      </c>
+      <c r="C41">
+        <v>2020</v>
+      </c>
+      <c r="D41" t="s">
+        <v>207</v>
+      </c>
+      <c r="E41" t="s">
+        <v>208</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Silvaspinosus_FernandezTriana"</v>
+      </c>
+      <c r="H41" t="s">
+        <v>209</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Silvaspinosus_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P41" t="s">
+        <v>211</v>
+      </c>
+      <c r="R41" t="s">
+        <v>210</v>
+      </c>
+      <c r="S41" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Silvaspinosus_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B42" t="s">
+        <v>208</v>
+      </c>
+      <c r="C42">
+        <v>2020</v>
+      </c>
+      <c r="D42" t="s">
+        <v>207</v>
+      </c>
+      <c r="E42" t="s">
+        <v>208</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Tobleronius_FernandezTriana"</v>
+      </c>
+      <c r="H42" t="s">
+        <v>209</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Tobleronius_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P42" t="s">
+        <v>211</v>
+      </c>
+      <c r="R42" t="s">
+        <v>210</v>
+      </c>
+      <c r="S42" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Tobleronius_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B43" t="s">
+        <v>208</v>
+      </c>
+      <c r="C43">
+        <v>2020</v>
+      </c>
+      <c r="D43" t="s">
+        <v>207</v>
+      </c>
+      <c r="E43" t="s">
+        <v>208</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Ungunicus_FernandezTriana"</v>
+      </c>
+      <c r="H43" t="s">
+        <v>209</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Ungunicus_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P43" t="s">
+        <v>211</v>
+      </c>
+      <c r="R43" t="s">
+        <v>210</v>
+      </c>
+      <c r="S43" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Ungunicus_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B44" t="s">
+        <v>208</v>
+      </c>
+      <c r="C44">
+        <v>2020</v>
+      </c>
+      <c r="D44" t="s">
+        <v>207</v>
+      </c>
+      <c r="E44" t="s">
+        <v>208</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Ypsilonogaster_FernandezTriana"</v>
+      </c>
+      <c r="H44" t="s">
+        <v>209</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Ypsilonogaster_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P44" t="s">
+        <v>211</v>
+      </c>
+      <c r="R44" t="s">
+        <v>210</v>
+      </c>
+      <c r="S44" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Ypsilonogaster_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B45" t="s">
+        <v>208</v>
+      </c>
+      <c r="C45">
+        <v>2020</v>
+      </c>
+      <c r="D45" t="s">
+        <v>207</v>
+      </c>
+      <c r="E45" t="s">
+        <v>208</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>"2020.Zachterbergius_FernandezTriana"</v>
+      </c>
+      <c r="H45" t="s">
+        <v>209</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="1"/>
+        <v>"2020.Zachterbergius_FernandezTriana" -&gt; "2020.Microgastrine"</v>
+      </c>
+      <c r="P45" t="s">
+        <v>211</v>
+      </c>
+      <c r="R45" t="s">
+        <v>210</v>
+      </c>
+      <c r="S45" t="str">
+        <f t="shared" si="2"/>
+        <v>"2020.Microgastrine" -&gt; "2020.Zachterbergius_FernandezTriana" [dir=back]</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>